<commit_message>
Modified doc files to accomodate new commands available from host
</commit_message>
<xml_diff>
--- a/doc/can_messages.xlsx
+++ b/doc/can_messages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="171">
   <si>
     <t>ID</t>
   </si>
@@ -393,18 +393,12 @@
     <t>300</t>
   </si>
   <si>
-    <t>32 values received ok, start write</t>
-  </si>
-  <si>
     <t>400</t>
   </si>
   <si>
     <t>FF</t>
   </si>
   <si>
-    <t>flash write successful, ready</t>
-  </si>
-  <si>
     <t>2FF</t>
   </si>
   <si>
@@ -433,6 +427,108 @@
   </si>
   <si>
     <t>06</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>Reset current frame</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>2E</t>
+  </si>
+  <si>
+    <t>9C</t>
+  </si>
+  <si>
+    <t>32 val received, CRC [frame nr, 1s tbyte, 2nd byte)</t>
+  </si>
+  <si>
+    <t>flash write successful, [frame nr]</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>40</t>
   </si>
 </sst>
 </file>
@@ -478,7 +574,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -718,11 +814,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -752,12 +861,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -769,6 +872,13 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1063,10 +1173,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V41"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1085,7 +1195,7 @@
     <col min="16" max="16" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="21" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="43.140625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="45.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1104,7 +1214,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="7"/>
       <c r="L1" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -1129,85 +1239,85 @@
       <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="28"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="39"/>
       <c r="L2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="27" t="s">
+      <c r="N2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="28"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="39"/>
       <c r="V2" s="14"/>
     </row>
     <row r="3" spans="1:22" s="25" customFormat="1">
-      <c r="A3" s="35">
-        <v>1</v>
-      </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="35" t="s">
+      <c r="A3" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="N3" s="36" t="s">
+      <c r="M3" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="36" t="s">
+      <c r="O3" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="36" t="s">
+      <c r="P3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="36" t="s">
+      <c r="Q3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="36" t="s">
+      <c r="R3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="S3" s="36" t="s">
+      <c r="S3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="T3" s="36" t="s">
+      <c r="T3" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="U3" s="37" t="s">
+      <c r="U3" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="V3" s="38" t="s">
+      <c r="V3" s="36" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:22" s="16" customFormat="1">
-      <c r="A4" s="17">
-        <v>2</v>
+      <c r="A4" s="17" t="s">
+        <v>146</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>3</v>
@@ -1238,8 +1348,8 @@
       </c>
     </row>
     <row r="5" spans="1:22" s="16" customFormat="1">
-      <c r="A5" s="17">
-        <v>3</v>
+      <c r="A5" s="17" t="s">
+        <v>139</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>16</v>
@@ -1277,324 +1387,316 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
-      <c r="A6" s="10">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="1:22" s="16" customFormat="1">
+      <c r="A6" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="20" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L7" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N6" s="2" t="s">
+      <c r="M7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="S6" s="2" t="s">
+      <c r="S7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="T7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U6" s="11" t="s">
+      <c r="U7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="V6" s="15" t="s">
+      <c r="V7" s="15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
-      <c r="A7" s="10">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
+    <row r="8" spans="1:22">
+      <c r="A8" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L8" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N7" s="2" t="s">
+      <c r="M8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="Q8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="R8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="S7" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="T7" s="2" t="s">
+      <c r="T8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="U7" s="11" t="s">
+      <c r="U8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="V7" s="15" t="s">
+      <c r="V8" s="15" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
-      <c r="A8" s="10">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
+    <row r="9" spans="1:22">
+      <c r="A9" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K9" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L9" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N8" s="2" t="s">
+      <c r="M9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="P9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="Q9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="R9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="S9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="T8" s="2" t="s">
+      <c r="T9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="U8" s="11" t="s">
+      <c r="U9" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="V8" s="15" t="s">
+      <c r="V9" s="15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
-      <c r="A9" s="10">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
+    <row r="10" spans="1:22">
+      <c r="A10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K10" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="L10" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="M9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N9" s="2" t="s">
+      <c r="M10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="Q10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="R9" s="2" t="s">
+      <c r="R10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="S9" s="2" t="s">
+      <c r="S10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="T9" s="2" t="s">
+      <c r="T10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="U9" s="11" t="s">
+      <c r="U10" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="V9" s="15" t="s">
+      <c r="V10" s="15" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
-      <c r="A10" s="10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
+    <row r="11" spans="1:22">
+      <c r="A11" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
-      <c r="A11" s="10">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>4</v>
@@ -1610,7 +1712,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="11"/>
       <c r="L11" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>4</v>
@@ -1626,15 +1728,15 @@
       <c r="T11" s="2"/>
       <c r="U11" s="11"/>
       <c r="V11" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:22">
-      <c r="A12" s="10">
-        <v>10</v>
+      <c r="A12" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>4</v>
@@ -1650,7 +1752,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="11"/>
       <c r="L12" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>4</v>
@@ -1666,15 +1768,15 @@
       <c r="T12" s="2"/>
       <c r="U12" s="11"/>
       <c r="V12" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:22">
-      <c r="A13" s="10">
-        <v>11</v>
+      <c r="A13" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>4</v>
@@ -1690,7 +1792,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="11"/>
       <c r="L13" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>4</v>
@@ -1706,15 +1808,15 @@
       <c r="T13" s="2"/>
       <c r="U13" s="11"/>
       <c r="V13" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:22">
-      <c r="A14" s="10">
-        <v>12</v>
+      <c r="A14" s="10" t="s">
+        <v>151</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>4</v>
@@ -1730,7 +1832,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="11"/>
       <c r="L14" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>4</v>
@@ -1746,15 +1848,15 @@
       <c r="T14" s="2"/>
       <c r="U14" s="11"/>
       <c r="V14" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:22">
-      <c r="A15" s="10">
-        <v>13</v>
+      <c r="A15" s="10" t="s">
+        <v>152</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>4</v>
@@ -1770,7 +1872,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="11"/>
       <c r="L15" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>4</v>
@@ -1786,15 +1888,15 @@
       <c r="T15" s="2"/>
       <c r="U15" s="11"/>
       <c r="V15" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:22">
-      <c r="A16" s="10">
-        <v>14</v>
+      <c r="A16" s="10" t="s">
+        <v>140</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>4</v>
@@ -1810,7 +1912,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="11"/>
       <c r="L16" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>4</v>
@@ -1826,15 +1928,15 @@
       <c r="T16" s="2"/>
       <c r="U16" s="11"/>
       <c r="V16" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:22">
-      <c r="A17" s="10">
-        <v>15</v>
+      <c r="A17" s="10" t="s">
+        <v>153</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>4</v>
@@ -1850,7 +1952,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="11"/>
       <c r="L17" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>4</v>
@@ -1866,15 +1968,15 @@
       <c r="T17" s="2"/>
       <c r="U17" s="11"/>
       <c r="V17" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:22">
-      <c r="A18" s="10">
-        <v>16</v>
+      <c r="A18" s="10" t="s">
+        <v>154</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>4</v>
@@ -1890,7 +1992,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="11"/>
       <c r="L18" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>4</v>
@@ -1906,15 +2008,15 @@
       <c r="T18" s="2"/>
       <c r="U18" s="11"/>
       <c r="V18" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:22">
-      <c r="A19" s="10">
-        <v>17</v>
+      <c r="A19" s="10" t="s">
+        <v>155</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>4</v>
@@ -1930,7 +2032,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="11"/>
       <c r="L19" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>4</v>
@@ -1946,15 +2048,15 @@
       <c r="T19" s="2"/>
       <c r="U19" s="11"/>
       <c r="V19" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:22">
-      <c r="A20" s="10">
-        <v>18</v>
+      <c r="A20" s="10" t="s">
+        <v>156</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>4</v>
@@ -1970,7 +2072,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="11"/>
       <c r="L20" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>4</v>
@@ -1986,15 +2088,15 @@
       <c r="T20" s="2"/>
       <c r="U20" s="11"/>
       <c r="V20" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:22">
-      <c r="A21" s="10">
-        <v>19</v>
+      <c r="A21" s="10" t="s">
+        <v>157</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>4</v>
@@ -2010,7 +2112,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="11"/>
       <c r="L21" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>4</v>
@@ -2026,15 +2128,15 @@
       <c r="T21" s="2"/>
       <c r="U21" s="11"/>
       <c r="V21" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="10">
-        <v>20</v>
+      <c r="A22" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>4</v>
@@ -2050,7 +2152,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="11"/>
       <c r="L22" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>4</v>
@@ -2066,15 +2168,15 @@
       <c r="T22" s="2"/>
       <c r="U22" s="11"/>
       <c r="V22" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:22">
-      <c r="A23" s="10">
-        <v>21</v>
+      <c r="A23" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>4</v>
@@ -2090,7 +2192,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="11"/>
       <c r="L23" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>4</v>
@@ -2106,15 +2208,15 @@
       <c r="T23" s="2"/>
       <c r="U23" s="11"/>
       <c r="V23" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:22">
-      <c r="A24" s="10">
-        <v>22</v>
+      <c r="A24" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>4</v>
@@ -2130,7 +2232,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="11"/>
       <c r="L24" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>4</v>
@@ -2146,15 +2248,15 @@
       <c r="T24" s="2"/>
       <c r="U24" s="11"/>
       <c r="V24" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:22">
-      <c r="A25" s="10">
-        <v>23</v>
+      <c r="A25" s="10" t="s">
+        <v>158</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>4</v>
@@ -2170,7 +2272,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="11"/>
       <c r="L25" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>4</v>
@@ -2186,15 +2288,15 @@
       <c r="T25" s="2"/>
       <c r="U25" s="11"/>
       <c r="V25" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:22">
-      <c r="A26" s="10">
-        <v>24</v>
+      <c r="A26" s="10" t="s">
+        <v>159</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>4</v>
@@ -2210,7 +2312,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="11"/>
       <c r="L26" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>4</v>
@@ -2226,15 +2328,15 @@
       <c r="T26" s="2"/>
       <c r="U26" s="11"/>
       <c r="V26" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:22">
-      <c r="A27" s="10">
-        <v>25</v>
+      <c r="A27" s="10" t="s">
+        <v>160</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>4</v>
@@ -2250,7 +2352,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="11"/>
       <c r="L27" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>4</v>
@@ -2266,15 +2368,15 @@
       <c r="T27" s="2"/>
       <c r="U27" s="11"/>
       <c r="V27" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="10">
-        <v>26</v>
+      <c r="A28" s="10" t="s">
+        <v>161</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>4</v>
@@ -2290,7 +2392,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="11"/>
       <c r="L28" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>4</v>
@@ -2306,15 +2408,15 @@
       <c r="T28" s="2"/>
       <c r="U28" s="11"/>
       <c r="V28" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:22">
-      <c r="A29" s="10">
-        <v>27</v>
+      <c r="A29" s="10" t="s">
+        <v>162</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>4</v>
@@ -2330,7 +2432,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="11"/>
       <c r="L29" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>4</v>
@@ -2346,15 +2448,15 @@
       <c r="T29" s="2"/>
       <c r="U29" s="11"/>
       <c r="V29" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:22">
-      <c r="A30" s="10">
-        <v>28</v>
+      <c r="A30" s="10" t="s">
+        <v>163</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>4</v>
@@ -2370,7 +2472,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="11"/>
       <c r="L30" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>4</v>
@@ -2386,15 +2488,15 @@
       <c r="T30" s="2"/>
       <c r="U30" s="11"/>
       <c r="V30" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:22">
-      <c r="A31" s="10">
-        <v>29</v>
+      <c r="A31" s="10" t="s">
+        <v>164</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>4</v>
@@ -2410,7 +2512,7 @@
       <c r="J31" s="2"/>
       <c r="K31" s="11"/>
       <c r="L31" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>4</v>
@@ -2426,15 +2528,15 @@
       <c r="T31" s="2"/>
       <c r="U31" s="11"/>
       <c r="V31" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:22">
-      <c r="A32" s="10">
-        <v>30</v>
+      <c r="A32" s="10" t="s">
+        <v>165</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>4</v>
@@ -2450,7 +2552,7 @@
       <c r="J32" s="2"/>
       <c r="K32" s="11"/>
       <c r="L32" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>4</v>
@@ -2466,15 +2568,15 @@
       <c r="T32" s="2"/>
       <c r="U32" s="11"/>
       <c r="V32" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:22">
-      <c r="A33" s="10">
-        <v>31</v>
+      <c r="A33" s="10" t="s">
+        <v>166</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>4</v>
@@ -2490,7 +2592,7 @@
       <c r="J33" s="2"/>
       <c r="K33" s="11"/>
       <c r="L33" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>4</v>
@@ -2506,15 +2608,15 @@
       <c r="T33" s="2"/>
       <c r="U33" s="11"/>
       <c r="V33" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:22">
-      <c r="A34" s="10">
-        <v>32</v>
+      <c r="A34" s="10" t="s">
+        <v>167</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>4</v>
@@ -2530,7 +2632,7 @@
       <c r="J34" s="2"/>
       <c r="K34" s="11"/>
       <c r="L34" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>4</v>
@@ -2546,15 +2648,15 @@
       <c r="T34" s="2"/>
       <c r="U34" s="11"/>
       <c r="V34" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:22">
-      <c r="A35" s="10">
-        <v>33</v>
+      <c r="A35" s="10" t="s">
+        <v>90</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>4</v>
@@ -2570,7 +2672,7 @@
       <c r="J35" s="2"/>
       <c r="K35" s="11"/>
       <c r="L35" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>4</v>
@@ -2586,15 +2688,15 @@
       <c r="T35" s="2"/>
       <c r="U35" s="11"/>
       <c r="V35" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:22">
-      <c r="A36" s="10">
-        <v>34</v>
+      <c r="A36" s="10" t="s">
+        <v>168</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>4</v>
@@ -2610,7 +2712,7 @@
       <c r="J36" s="2"/>
       <c r="K36" s="11"/>
       <c r="L36" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>4</v>
@@ -2626,15 +2728,15 @@
       <c r="T36" s="2"/>
       <c r="U36" s="11"/>
       <c r="V36" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:22">
-      <c r="A37" s="10">
-        <v>35</v>
+      <c r="A37" s="10" t="s">
+        <v>169</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>4</v>
@@ -2650,7 +2752,7 @@
       <c r="J37" s="2"/>
       <c r="K37" s="11"/>
       <c r="L37" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M37" s="2" t="s">
         <v>4</v>
@@ -2666,46 +2768,52 @@
       <c r="T37" s="2"/>
       <c r="U37" s="11"/>
       <c r="V37" s="15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22">
+      <c r="A38" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="11"/>
+      <c r="V38" s="15" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="38" spans="1:22" s="25" customFormat="1">
-      <c r="A38" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="M38" s="22">
-        <v>1</v>
-      </c>
-      <c r="N38" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="O38" s="22"/>
-      <c r="P38" s="22"/>
-      <c r="Q38" s="22"/>
-      <c r="R38" s="22"/>
-      <c r="S38" s="22"/>
-      <c r="T38" s="22"/>
-      <c r="U38" s="23"/>
-      <c r="V38" s="24" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:22" s="25" customFormat="1">
       <c r="A39" s="21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
@@ -2718,99 +2826,137 @@
       <c r="J39" s="22"/>
       <c r="K39" s="23"/>
       <c r="L39" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="M39" s="22">
-        <v>1</v>
-      </c>
-      <c r="N39" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="O39" s="22"/>
-      <c r="P39" s="22"/>
+        <v>124</v>
+      </c>
+      <c r="M39" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="N39" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="O39" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="P39" s="22" t="s">
+        <v>140</v>
+      </c>
       <c r="Q39" s="22"/>
       <c r="R39" s="22"/>
       <c r="S39" s="22"/>
       <c r="T39" s="22"/>
       <c r="U39" s="23"/>
       <c r="V39" s="24" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22" s="16" customFormat="1">
-      <c r="A40" s="17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" s="25" customFormat="1">
+      <c r="A40" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="23"/>
+      <c r="L40" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="M40" s="22">
+        <v>1</v>
+      </c>
+      <c r="N40" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="O40" s="22"/>
+      <c r="P40" s="22"/>
+      <c r="Q40" s="22"/>
+      <c r="R40" s="22"/>
+      <c r="S40" s="22"/>
+      <c r="T40" s="22"/>
+      <c r="U40" s="23"/>
+      <c r="V40" s="24" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" s="16" customFormat="1">
+      <c r="A41" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B41" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C41" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="M40" s="18">
+      <c r="D41" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="M41" s="18">
         <v>3</v>
       </c>
-      <c r="N40" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="O40" s="18" t="s">
+      <c r="N41" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="O41" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="P40" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
-      <c r="T40" s="18"/>
-      <c r="U40" s="19"/>
-      <c r="V40" s="39" t="s">
+      <c r="P41" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
+      <c r="T41" s="18"/>
+      <c r="U41" s="19"/>
+      <c r="V41" s="37" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" s="16" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A42" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="B42" s="28" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="41" spans="1:22" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A41" s="29" t="s">
+      <c r="C42" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="30"/>
+      <c r="O42" s="28"/>
+      <c r="P42" s="28"/>
+      <c r="Q42" s="28"/>
+      <c r="R42" s="28"/>
+      <c r="S42" s="28"/>
+      <c r="T42" s="28"/>
+      <c r="U42" s="29"/>
+      <c r="V42" s="31" t="s">
         <v>134</v>
-      </c>
-      <c r="B41" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="C41" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="30"/>
-      <c r="I41" s="30"/>
-      <c r="J41" s="30"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="29"/>
-      <c r="M41" s="30"/>
-      <c r="N41" s="32"/>
-      <c r="O41" s="30"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="30"/>
-      <c r="S41" s="30"/>
-      <c r="T41" s="30"/>
-      <c r="U41" s="31"/>
-      <c r="V41" s="33" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2819,7 +2965,7 @@
     <mergeCell ref="N2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="67" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="66" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>